<commit_message>
done with practice with excel
</commit_message>
<xml_diff>
--- a/LibraryCT.xlsx
+++ b/LibraryCT.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beka\IdeaProjects\All_US_For_LibraryCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50EDF6A-D72D-46F1-9588-038804B2C6D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CDE1C7-27C5-408B-B52B-31EFF020FEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2444527-0996-41AF-A7FB-D6AFFEACD96D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="120">
   <si>
     <t>Execute</t>
   </si>
@@ -84,102 +84,6 @@
     <t>http://library2.cybertekschool.com/login.html</t>
   </si>
   <si>
-    <t>student136@library</t>
-  </si>
-  <si>
-    <t>student137@library</t>
-  </si>
-  <si>
-    <t>student138@library</t>
-  </si>
-  <si>
-    <t>librarian67@library</t>
-  </si>
-  <si>
-    <t>oKpgJXle</t>
-  </si>
-  <si>
-    <t>o6JnXwlf</t>
-  </si>
-  <si>
-    <t>QiAdgS4z</t>
-  </si>
-  <si>
-    <t>5ktpB2e5</t>
-  </si>
-  <si>
-    <t>student139@library</t>
-  </si>
-  <si>
-    <t>student140@library</t>
-  </si>
-  <si>
-    <t>student141@library</t>
-  </si>
-  <si>
-    <t>librarian68@library</t>
-  </si>
-  <si>
-    <t>student142@library</t>
-  </si>
-  <si>
-    <t>student143@library</t>
-  </si>
-  <si>
-    <t>student144@library</t>
-  </si>
-  <si>
-    <t>librarian69@library</t>
-  </si>
-  <si>
-    <t>student145@library</t>
-  </si>
-  <si>
-    <t>student146@library</t>
-  </si>
-  <si>
-    <t>student147@library</t>
-  </si>
-  <si>
-    <t>librarian65@library</t>
-  </si>
-  <si>
-    <t>OsU5XYlm</t>
-  </si>
-  <si>
-    <t>oyoBB50n</t>
-  </si>
-  <si>
-    <t>Y8IGg0Iy</t>
-  </si>
-  <si>
-    <t>hsTpIdzm</t>
-  </si>
-  <si>
-    <t>FJBph6oV</t>
-  </si>
-  <si>
-    <t>HziugPen</t>
-  </si>
-  <si>
-    <t>LutHHgbl</t>
-  </si>
-  <si>
-    <t>KNPXrm3S</t>
-  </si>
-  <si>
-    <t>TbyqniAP</t>
-  </si>
-  <si>
-    <t>YpQScANR</t>
-  </si>
-  <si>
-    <t>uyO7tdDI</t>
-  </si>
-  <si>
-    <t>E2sjHRff</t>
-  </si>
-  <si>
     <t>student30@library</t>
   </si>
   <si>
@@ -469,13 +373,35 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>PASS!!</t>
+  </si>
+  <si>
+    <t>01:59 PM</t>
+  </si>
+  <si>
+    <t>02:00 PM</t>
+  </si>
+  <si>
+    <t>02:01 PM</t>
+  </si>
+  <si>
+    <t>09:04 PM</t>
+  </si>
+  <si>
+    <t>09:05 PM</t>
+  </si>
+  <si>
+    <t>09:06 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,19 +418,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF305496"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
-      <color rgb="FF305496"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF305496"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -572,31 +486,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -914,18 +816,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CEDE1-6066-442D-A0A6-84C8A911F59B}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="20.109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="16.88671875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="40.21875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="39.5546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -948,960 +850,1203 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.2" thickBot="1">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.2" thickBot="1">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>137</v>
+      <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16.2" thickBot="1">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>139</v>
+      <c r="B7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.2" thickBot="1">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>141</v>
+      <c r="B8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.2" thickBot="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>143</v>
+      <c r="B9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="24" thickBot="1">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" thickBot="1">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24" thickBot="1">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="24" thickBot="1">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="24" thickBot="1">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="24" thickBot="1">
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.2" thickBot="1">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="24" thickBot="1">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="24" thickBot="1">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="24" thickBot="1">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="24" thickBot="1">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="24" thickBot="1">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="24" thickBot="1">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="24" thickBot="1">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="24" thickBot="1">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="24" thickBot="1">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="24" thickBot="1">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16.2" thickBot="1">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="24" thickBot="1">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.2" thickBot="1">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.2" thickBot="1">
       <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16.2" thickBot="1">
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16.2" thickBot="1">
       <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.2" thickBot="1">
       <c r="A30" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16.2" thickBot="1">
       <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16.2" thickBot="1">
       <c r="A32" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.2" thickBot="1">
       <c r="A33" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16.2" thickBot="1">
       <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16.2" thickBot="1">
       <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16.2" thickBot="1">
       <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16.2" thickBot="1">
       <c r="A37" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16.2" thickBot="1">
       <c r="A38" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>113</v>
+      </c>
+      <c r="G38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16.2" thickBot="1">
       <c r="A39" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16.2" thickBot="1">
       <c r="A40" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16.2" thickBot="1">
       <c r="A41" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16.2" thickBot="1">
       <c r="A42" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>113</v>
+      </c>
+      <c r="G42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="16.2" thickBot="1">
       <c r="A43" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="16.2" thickBot="1">
       <c r="A44" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16.2" thickBot="1">
       <c r="A45" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16.2" thickBot="1">
       <c r="A46" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="16.2" thickBot="1">
       <c r="A47" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="16.2" thickBot="1">
       <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>113</v>
+      </c>
+      <c r="G48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="16.2" thickBot="1">
       <c r="A49" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="16.2" thickBot="1">
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="16.2" thickBot="1">
       <c r="A50" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="16.2" thickBot="1">
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="16.2" thickBot="1">
       <c r="A51" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16.2" thickBot="1">
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16.2" thickBot="1">
       <c r="A52" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16.2" thickBot="1">
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16.2" thickBot="1">
       <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A59" t="s">
-        <v>1</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="7" t="s">
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" t="s">
         <v>119</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A63" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A64" t="s">
-        <v>1</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A67" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A69" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1914,69 +2059,52 @@
     <hyperlink ref="D3" r:id="rId6" xr:uid="{753D7B1D-7125-4337-B028-33C00AFF5781}"/>
     <hyperlink ref="D4" r:id="rId7" xr:uid="{E4E5FB16-B3BB-4157-B676-B500C85C172D}"/>
     <hyperlink ref="D5" r:id="rId8" xr:uid="{5C324E2E-C495-4AC6-B7A4-4262A1F0FAA8}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{DBFD0B2E-120B-4EBB-BB57-E8518205F644}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{1D5FD287-C45B-46B6-8C34-1BB42C8E41C9}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{63254AD4-80FE-4F38-B9DF-96B40A3313C2}"/>
-    <hyperlink ref="D8" r:id="rId12" xr:uid="{6A54584E-AB8B-4E79-8F16-7D18E7078241}"/>
-    <hyperlink ref="D9" r:id="rId13" xr:uid="{8773F3F7-6671-44B3-BB8B-4D2A72081385}"/>
-    <hyperlink ref="D10" r:id="rId14" xr:uid="{2AD46C4A-037B-46DE-8090-2CF9D895BA61}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{9DC59AEA-33A8-4247-9B15-B34CD68F0550}"/>
-    <hyperlink ref="D12" r:id="rId16" xr:uid="{CC05E17D-F162-466B-94BC-AEBC79EECA01}"/>
-    <hyperlink ref="D13" r:id="rId17" xr:uid="{8125FF87-2851-49AE-98F3-58BE790ED0EA}"/>
-    <hyperlink ref="D14" r:id="rId18" xr:uid="{096F9B5A-D761-4E88-99CE-D57D8F592085}"/>
-    <hyperlink ref="D15" r:id="rId19" xr:uid="{5B7B5C3D-74AD-412A-BAA5-25B10B7285B8}"/>
-    <hyperlink ref="D16" r:id="rId20" xr:uid="{8972748C-BF2C-4C48-BC98-15F586C5C2FF}"/>
-    <hyperlink ref="D17" r:id="rId21" xr:uid="{5744B630-3F25-4C8F-9928-35C0F22F6ACA}"/>
-    <hyperlink ref="D18" r:id="rId22" xr:uid="{DCB13309-4AFC-4ED6-97F3-B791C81F622A}"/>
-    <hyperlink ref="D19" r:id="rId23" xr:uid="{56FB3E6E-F6D1-4402-A2DB-0ED5267C4AAE}"/>
-    <hyperlink ref="D20" r:id="rId24" xr:uid="{14ADCF73-EC0C-4CE6-A7B0-E908F7EB6225}"/>
-    <hyperlink ref="D21" r:id="rId25" xr:uid="{9C6DE0FB-8536-4389-A9FF-1B1A8470787A}"/>
-    <hyperlink ref="D22" r:id="rId26" xr:uid="{9EFA201F-B392-4302-87DC-4A88546E8BD2}"/>
-    <hyperlink ref="D23" r:id="rId27" xr:uid="{95909F8B-DCB2-42B4-AA63-F72A983E3702}"/>
-    <hyperlink ref="D24" r:id="rId28" xr:uid="{037CF158-A1FB-49E2-9307-CFB6C8F9EEF9}"/>
-    <hyperlink ref="D25" r:id="rId29" xr:uid="{24FB4042-6945-4D8C-9D05-5C88920AF1DA}"/>
-    <hyperlink ref="D26" r:id="rId30" xr:uid="{2DFC75D2-1EC4-48CC-B962-B9211A22FCB0}"/>
-    <hyperlink ref="D27" r:id="rId31" xr:uid="{8F01A734-97F5-4CA9-9A79-076DFB2613EB}"/>
-    <hyperlink ref="D28" r:id="rId32" xr:uid="{3A89B1AC-9719-49AE-AAC3-527AB238411D}"/>
-    <hyperlink ref="D29" r:id="rId33" xr:uid="{0D240F85-B4DE-4020-AB14-FB31E0E012AD}"/>
-    <hyperlink ref="D30" r:id="rId34" xr:uid="{A3C97BB7-9CF7-426B-A1C0-21A901EF2024}"/>
-    <hyperlink ref="D31" r:id="rId35" xr:uid="{B892FBD0-4AF4-46AA-9F9A-203DC902259C}"/>
-    <hyperlink ref="D32" r:id="rId36" xr:uid="{BD509B62-8552-4369-8190-1CDF818685AE}"/>
-    <hyperlink ref="D33" r:id="rId37" xr:uid="{16AB535D-55FC-477E-B158-ED5E6A1BFD56}"/>
-    <hyperlink ref="D34" r:id="rId38" xr:uid="{19019418-7994-4A91-A16D-89310099F26F}"/>
-    <hyperlink ref="D35" r:id="rId39" xr:uid="{CAC0030B-0C07-4C51-B7BD-AB2497DDE881}"/>
-    <hyperlink ref="D36" r:id="rId40" xr:uid="{DC3A1520-9B12-420B-A031-EAF66432BECB}"/>
-    <hyperlink ref="D37" r:id="rId41" xr:uid="{C48A7BD8-501C-4DE2-95BC-D40D94EEEF88}"/>
-    <hyperlink ref="D38" r:id="rId42" xr:uid="{80B48FB8-8F75-4CB9-8A7F-A315D706286F}"/>
-    <hyperlink ref="D39" r:id="rId43" xr:uid="{F4307200-838B-419F-9B4D-2D0D1DD4D242}"/>
-    <hyperlink ref="D40" r:id="rId44" xr:uid="{C7FF786B-A88F-4BAC-97BA-847EDBA5DD98}"/>
-    <hyperlink ref="D41" r:id="rId45" xr:uid="{B4034D58-912F-4491-AD10-0CECCA551541}"/>
-    <hyperlink ref="D42" r:id="rId46" xr:uid="{7BA9E8EC-8147-47EF-A590-C9E6A06BDEC4}"/>
-    <hyperlink ref="D43" r:id="rId47" xr:uid="{1018EB8E-E22F-46C8-8B48-21D840F739E3}"/>
-    <hyperlink ref="D44" r:id="rId48" xr:uid="{9C03DE6B-CAAC-4180-AFEC-38A78B80BDE0}"/>
-    <hyperlink ref="D45" r:id="rId49" xr:uid="{FDAB12C6-7E7D-4E3E-965B-51589AE15C3A}"/>
-    <hyperlink ref="D46" r:id="rId50" xr:uid="{63CDE962-A44D-4E6A-AA3E-080AB96536EA}"/>
-    <hyperlink ref="D47" r:id="rId51" xr:uid="{58A973F9-13E9-467C-9431-AD9E2BABBA62}"/>
-    <hyperlink ref="D48" r:id="rId52" xr:uid="{C6080667-7125-4D21-AEE8-708FCE0FA1E0}"/>
-    <hyperlink ref="D49" r:id="rId53" xr:uid="{3FD49FFA-EC88-40AE-953A-97088AB86F3A}"/>
-    <hyperlink ref="D50" r:id="rId54" xr:uid="{D444434B-4DE1-464E-93FF-60446867C952}"/>
-    <hyperlink ref="D51" r:id="rId55" xr:uid="{D6DA2E44-1B86-4E22-AA5A-93B98E5E6899}"/>
-    <hyperlink ref="D52" r:id="rId56" xr:uid="{5FF576AE-435A-4207-93FC-9DAC12BB3E10}"/>
-    <hyperlink ref="D53" r:id="rId57" xr:uid="{02295CE9-6CB1-49C4-ABEF-8574C350EF9E}"/>
-    <hyperlink ref="D54" r:id="rId58" xr:uid="{92AA27ED-64FA-439D-8172-971C60D80F14}"/>
-    <hyperlink ref="D55" r:id="rId59" xr:uid="{59872904-1487-45EA-B00C-726114EC320E}"/>
-    <hyperlink ref="D56" r:id="rId60" xr:uid="{135C2520-CC7C-48CB-9C30-FB1994588108}"/>
-    <hyperlink ref="D57" r:id="rId61" xr:uid="{8E432747-83F6-485E-9205-0FD2C881CF5C}"/>
-    <hyperlink ref="D58" r:id="rId62" xr:uid="{C3891B75-F15B-4400-A5BA-4BD37A6182EC}"/>
-    <hyperlink ref="D59" r:id="rId63" xr:uid="{9C811B08-E29A-40FA-9FB2-0F3BEAAE2125}"/>
-    <hyperlink ref="D60" r:id="rId64" xr:uid="{36E679FA-4AEF-4997-8C8B-5D7FB4B66D93}"/>
-    <hyperlink ref="D61" r:id="rId65" xr:uid="{8D8B2663-589D-4A33-97AE-2AAD49F8B380}"/>
-    <hyperlink ref="D62" r:id="rId66" xr:uid="{1BD7B30C-A31B-452F-8F12-6C6CB7AFFE78}"/>
-    <hyperlink ref="D63" r:id="rId67" xr:uid="{494A19E6-5033-4FA3-B247-58A49C77D5B1}"/>
-    <hyperlink ref="D64" r:id="rId68" xr:uid="{6D936CDE-C1DE-4C19-A3C8-A77E5C8126C3}"/>
-    <hyperlink ref="D65" r:id="rId69" xr:uid="{65081682-5ADA-4D62-9A33-AB3150712B11}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{1D5FD287-C45B-46B6-8C34-1BB42C8E41C9}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{63254AD4-80FE-4F38-B9DF-96B40A3313C2}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{6A54584E-AB8B-4E79-8F16-7D18E7078241}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{8773F3F7-6671-44B3-BB8B-4D2A72081385}"/>
+    <hyperlink ref="D10" r:id="rId13" xr:uid="{2DFC75D2-1EC4-48CC-B962-B9211A22FCB0}"/>
+    <hyperlink ref="D11" r:id="rId14" xr:uid="{8F01A734-97F5-4CA9-9A79-076DFB2613EB}"/>
+    <hyperlink ref="D12" r:id="rId15" xr:uid="{3A89B1AC-9719-49AE-AAC3-527AB238411D}"/>
+    <hyperlink ref="D13" r:id="rId16" xr:uid="{0D240F85-B4DE-4020-AB14-FB31E0E012AD}"/>
+    <hyperlink ref="D14" r:id="rId17" xr:uid="{A3C97BB7-9CF7-426B-A1C0-21A901EF2024}"/>
+    <hyperlink ref="D15" r:id="rId18" xr:uid="{B892FBD0-4AF4-46AA-9F9A-203DC902259C}"/>
+    <hyperlink ref="D16" r:id="rId19" xr:uid="{BD509B62-8552-4369-8190-1CDF818685AE}"/>
+    <hyperlink ref="D17" r:id="rId20" xr:uid="{16AB535D-55FC-477E-B158-ED5E6A1BFD56}"/>
+    <hyperlink ref="D18" r:id="rId21" xr:uid="{19019418-7994-4A91-A16D-89310099F26F}"/>
+    <hyperlink ref="D19" r:id="rId22" xr:uid="{CAC0030B-0C07-4C51-B7BD-AB2497DDE881}"/>
+    <hyperlink ref="D20" r:id="rId23" xr:uid="{DC3A1520-9B12-420B-A031-EAF66432BECB}"/>
+    <hyperlink ref="D21" r:id="rId24" xr:uid="{C48A7BD8-501C-4DE2-95BC-D40D94EEEF88}"/>
+    <hyperlink ref="D22" r:id="rId25" xr:uid="{80B48FB8-8F75-4CB9-8A7F-A315D706286F}"/>
+    <hyperlink ref="D23" r:id="rId26" xr:uid="{F4307200-838B-419F-9B4D-2D0D1DD4D242}"/>
+    <hyperlink ref="D24" r:id="rId27" xr:uid="{C7FF786B-A88F-4BAC-97BA-847EDBA5DD98}"/>
+    <hyperlink ref="D25" r:id="rId28" xr:uid="{B4034D58-912F-4491-AD10-0CECCA551541}"/>
+    <hyperlink ref="D26" r:id="rId29" xr:uid="{7BA9E8EC-8147-47EF-A590-C9E6A06BDEC4}"/>
+    <hyperlink ref="D27" r:id="rId30" xr:uid="{1018EB8E-E22F-46C8-8B48-21D840F739E3}"/>
+    <hyperlink ref="D28" r:id="rId31" xr:uid="{9C03DE6B-CAAC-4180-AFEC-38A78B80BDE0}"/>
+    <hyperlink ref="D29" r:id="rId32" xr:uid="{FDAB12C6-7E7D-4E3E-965B-51589AE15C3A}"/>
+    <hyperlink ref="D30" r:id="rId33" xr:uid="{63CDE962-A44D-4E6A-AA3E-080AB96536EA}"/>
+    <hyperlink ref="D31" r:id="rId34" xr:uid="{58A973F9-13E9-467C-9431-AD9E2BABBA62}"/>
+    <hyperlink ref="D32" r:id="rId35" xr:uid="{C6080667-7125-4D21-AEE8-708FCE0FA1E0}"/>
+    <hyperlink ref="D33" r:id="rId36" xr:uid="{3FD49FFA-EC88-40AE-953A-97088AB86F3A}"/>
+    <hyperlink ref="D34" r:id="rId37" xr:uid="{D444434B-4DE1-464E-93FF-60446867C952}"/>
+    <hyperlink ref="D35" r:id="rId38" xr:uid="{D6DA2E44-1B86-4E22-AA5A-93B98E5E6899}"/>
+    <hyperlink ref="D36" r:id="rId39" xr:uid="{5FF576AE-435A-4207-93FC-9DAC12BB3E10}"/>
+    <hyperlink ref="D37" r:id="rId40" xr:uid="{02295CE9-6CB1-49C4-ABEF-8574C350EF9E}"/>
+    <hyperlink ref="D38" r:id="rId41" xr:uid="{92AA27ED-64FA-439D-8172-971C60D80F14}"/>
+    <hyperlink ref="D39" r:id="rId42" xr:uid="{59872904-1487-45EA-B00C-726114EC320E}"/>
+    <hyperlink ref="D40" r:id="rId43" xr:uid="{135C2520-CC7C-48CB-9C30-FB1994588108}"/>
+    <hyperlink ref="D41" r:id="rId44" xr:uid="{8E432747-83F6-485E-9205-0FD2C881CF5C}"/>
+    <hyperlink ref="D42" r:id="rId45" xr:uid="{C3891B75-F15B-4400-A5BA-4BD37A6182EC}"/>
+    <hyperlink ref="D43" r:id="rId46" xr:uid="{9C811B08-E29A-40FA-9FB2-0F3BEAAE2125}"/>
+    <hyperlink ref="D44" r:id="rId47" xr:uid="{36E679FA-4AEF-4997-8C8B-5D7FB4B66D93}"/>
+    <hyperlink ref="D45" r:id="rId48" xr:uid="{8D8B2663-589D-4A33-97AE-2AAD49F8B380}"/>
+    <hyperlink ref="D46" r:id="rId49" xr:uid="{1BD7B30C-A31B-452F-8F12-6C6CB7AFFE78}"/>
+    <hyperlink ref="D47" r:id="rId50" xr:uid="{494A19E6-5033-4FA3-B247-58A49C77D5B1}"/>
+    <hyperlink ref="D48" r:id="rId51" xr:uid="{6D936CDE-C1DE-4C19-A3C8-A77E5C8126C3}"/>
+    <hyperlink ref="D49" r:id="rId52" xr:uid="{65081682-5ADA-4D62-9A33-AB3150712B11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId70"/>
+  <pageSetup orientation="portrait" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>